<commit_message>
big chages. both getFacultyInfo() and getStudentInfo() methods now return the correct data in HTML format. Also, database has a lot of new entries added to it so we can search for students and faculty
</commit_message>
<xml_diff>
--- a/Group5_GanttChart.xlsx
+++ b/Group5_GanttChart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FA459C-C41D-4191-ABE8-865231B83B9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F3747-1402-4352-A3DA-5E1F4BB0EFEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -891,6 +891,48 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="11" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -898,48 +940,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -956,37 +956,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1113,15 +1083,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="totalRow" dxfId="9"/>
+      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="lastColumn" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1540,7 +1510,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE12" sqref="AE12"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1589,102 +1559,102 @@
         <v>30</v>
       </c>
       <c r="B3" s="60"/>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="82">
+      <c r="D3" s="91"/>
+      <c r="E3" s="89">
         <v>44292</v>
       </c>
-      <c r="F3" s="82"/>
+      <c r="F3" s="89"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="91"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="86">
         <f>I5</f>
         <v>44291</v>
       </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="79" t="s">
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="79" t="s">
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="79" t="s">
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="80"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="80"/>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="81"/>
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="86"/>
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="87"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="87"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="86"/>
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="87"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="86"/>
+      <c r="AZ4" s="87"/>
+      <c r="BA4" s="87"/>
+      <c r="BB4" s="87"/>
+      <c r="BC4" s="87"/>
+      <c r="BD4" s="87"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="86"/>
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="87"/>
+      <c r="BI4" s="87"/>
+      <c r="BJ4" s="87"/>
+      <c r="BK4" s="87"/>
+      <c r="BL4" s="88"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44291</v>
@@ -2326,8 +2296,8 @@
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
       <c r="L9" s="39"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="39"/>
       <c r="P9" s="39"/>
       <c r="Q9" s="39"/>
@@ -2409,9 +2379,9 @@
       <c r="L10" s="39"/>
       <c r="M10" s="39"/>
       <c r="N10" s="39"/>
-      <c r="O10" s="83"/>
-      <c r="P10" s="83"/>
-      <c r="Q10" s="85"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="78"/>
       <c r="R10" s="39"/>
       <c r="S10" s="39"/>
       <c r="T10" s="39"/>
@@ -2541,7 +2511,9 @@
       <c r="C12" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="27">
+        <v>1</v>
+      </c>
       <c r="E12" s="62">
         <v>44298</v>
       </c>
@@ -2557,12 +2529,12 @@
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
       <c r="O12" s="39"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="89"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
+      <c r="R12" s="83"/>
+      <c r="S12" s="83"/>
+      <c r="T12" s="83"/>
+      <c r="U12" s="82"/>
       <c r="V12" s="39"/>
       <c r="W12" s="39"/>
       <c r="X12" s="39"/>
@@ -2613,7 +2585,9 @@
         <v>47</v>
       </c>
       <c r="C13" s="67"/>
-      <c r="D13" s="27"/>
+      <c r="D13" s="27">
+        <v>0.5</v>
+      </c>
       <c r="E13" s="62">
         <v>44298</v>
       </c>
@@ -2629,14 +2603,14 @@
       <c r="M13" s="39"/>
       <c r="N13" s="39"/>
       <c r="O13" s="39"/>
-      <c r="P13" s="92"/>
-      <c r="Q13" s="92"/>
-      <c r="R13" s="92"/>
-      <c r="S13" s="92"/>
-      <c r="T13" s="92"/>
-      <c r="U13" s="86"/>
-      <c r="V13" s="86"/>
-      <c r="W13" s="86"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="79"/>
+      <c r="V13" s="79"/>
+      <c r="W13" s="79"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
@@ -2685,7 +2659,9 @@
         <v>48</v>
       </c>
       <c r="C14" s="67"/>
-      <c r="D14" s="27"/>
+      <c r="D14" s="27">
+        <v>1</v>
+      </c>
       <c r="E14" s="62">
         <v>44302</v>
       </c>
@@ -2705,13 +2681,13 @@
       <c r="Q14" s="39"/>
       <c r="R14" s="39"/>
       <c r="S14" s="39"/>
-      <c r="T14" s="91"/>
-      <c r="U14" s="91"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
-      <c r="X14" s="86"/>
-      <c r="Y14" s="86"/>
-      <c r="Z14" s="86"/>
+      <c r="T14" s="84"/>
+      <c r="U14" s="84"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
+      <c r="X14" s="79"/>
+      <c r="Y14" s="79"/>
+      <c r="Z14" s="79"/>
       <c r="AA14" s="39"/>
       <c r="AB14" s="39"/>
       <c r="AC14" s="39"/>
@@ -2853,12 +2829,12 @@
       <c r="W16" s="39"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="39"/>
-      <c r="Z16" s="84"/>
-      <c r="AA16" s="84"/>
-      <c r="AB16" s="84"/>
-      <c r="AC16" s="84"/>
-      <c r="AD16" s="84"/>
-      <c r="AE16" s="84"/>
+      <c r="Z16" s="77"/>
+      <c r="AA16" s="77"/>
+      <c r="AB16" s="77"/>
+      <c r="AC16" s="77"/>
+      <c r="AD16" s="77"/>
+      <c r="AE16" s="77"/>
       <c r="AF16" s="39"/>
       <c r="AG16" s="39"/>
       <c r="AH16" s="39"/>
@@ -2927,12 +2903,12 @@
       <c r="AB17" s="39"/>
       <c r="AC17" s="39"/>
       <c r="AD17" s="39"/>
-      <c r="AE17" s="88"/>
-      <c r="AF17" s="88"/>
-      <c r="AG17" s="88"/>
-      <c r="AH17" s="88"/>
-      <c r="AI17" s="88"/>
-      <c r="AJ17" s="88"/>
+      <c r="AE17" s="81"/>
+      <c r="AF17" s="81"/>
+      <c r="AG17" s="81"/>
+      <c r="AH17" s="81"/>
+      <c r="AI17" s="81"/>
+      <c r="AJ17" s="81"/>
       <c r="AK17" s="39"/>
       <c r="AL17" s="39"/>
       <c r="AM17" s="39"/>
@@ -3002,12 +2978,12 @@
       <c r="AH18" s="39"/>
       <c r="AI18" s="39"/>
       <c r="AJ18" s="39"/>
-      <c r="AK18" s="84"/>
-      <c r="AL18" s="84"/>
-      <c r="AM18" s="84"/>
-      <c r="AN18" s="84"/>
-      <c r="AO18" s="84"/>
-      <c r="AP18" s="84"/>
+      <c r="AK18" s="77"/>
+      <c r="AL18" s="77"/>
+      <c r="AM18" s="77"/>
+      <c r="AN18" s="77"/>
+      <c r="AO18" s="77"/>
+      <c r="AP18" s="77"/>
       <c r="AQ18" s="39"/>
       <c r="AR18" s="39"/>
       <c r="AS18" s="39"/>
@@ -3075,13 +3051,13 @@
       <c r="AL19" s="39"/>
       <c r="AM19" s="39"/>
       <c r="AN19" s="39"/>
-      <c r="AO19" s="86"/>
-      <c r="AP19" s="86"/>
-      <c r="AQ19" s="86"/>
-      <c r="AR19" s="86"/>
-      <c r="AS19" s="86"/>
-      <c r="AT19" s="86"/>
-      <c r="AU19" s="86"/>
+      <c r="AO19" s="79"/>
+      <c r="AP19" s="79"/>
+      <c r="AQ19" s="79"/>
+      <c r="AR19" s="79"/>
+      <c r="AS19" s="79"/>
+      <c r="AT19" s="79"/>
+      <c r="AU19" s="79"/>
       <c r="AV19" s="39"/>
       <c r="AW19" s="39"/>
       <c r="AX19" s="39"/>
@@ -3140,11 +3116,11 @@
       <c r="AH20" s="39"/>
       <c r="AI20" s="39"/>
       <c r="AJ20" s="39"/>
-      <c r="AK20" s="87"/>
-      <c r="AL20" s="87"/>
-      <c r="AM20" s="87"/>
-      <c r="AN20" s="87"/>
-      <c r="AO20" s="87"/>
+      <c r="AK20" s="80"/>
+      <c r="AL20" s="80"/>
+      <c r="AM20" s="80"/>
+      <c r="AN20" s="80"/>
+      <c r="AO20" s="80"/>
       <c r="AP20" s="39"/>
       <c r="AQ20" s="39"/>
       <c r="AR20" s="39"/>
@@ -3325,6 +3301,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -3332,11 +3313,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D22">
     <cfRule type="dataBar" priority="16">
@@ -3353,15 +3329,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL8 I11:BL11 I9:L9 O9:BL9 I10:N10 Q10:BL10 I12:O12 U12:BL12 I14:S14 X13:BL13 I13:T13 I15:BL15 AA14:BL14 I16:Y16 I17:AD17 AF16:BL16 AK17:BL17 I18:AJ18 I19:AN19 AV19:BL19 I20:AJ20 AP20:BL20 I21:BL22 AQ18:BL18">
-    <cfRule type="expression" dxfId="5" priority="35">
+    <cfRule type="expression" dxfId="2" priority="35">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL8 I11:BL11 I9:L9 O9:BL9 I10:N10 Q10:BL10 I12:O12 U12:BL12 I14:S14 X13:BL13 I13:T13 I15:BL15 AA14:BL14 I16:Y16 I17:AD17 AF16:BL16 AK17:BL17 I18:AJ18 I19:AN19 AV19:BL19 I20:AJ20 AP20:BL20 I21:BL22 AQ18:BL18">
-    <cfRule type="expression" dxfId="4" priority="29">
+    <cfRule type="expression" dxfId="1" priority="29">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="30" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>